<commit_message>
made changes to driver script and added new java class.
</commit_message>
<xml_diff>
--- a/Maven_Automation/TestData/DWHomePage.xlsx
+++ b/Maven_Automation/TestData/DWHomePage.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="HomePage" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="NewsArticle" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="46">
   <si>
     <t>RunTestCase</t>
   </si>
@@ -45,9 +45,6 @@
     <t>Passowrd</t>
   </si>
   <si>
-    <t>Post the comment through selenium script, edit the script and like the post</t>
-  </si>
-  <si>
     <t>Microblog_Comment</t>
   </si>
   <si>
@@ -64,6 +61,99 @@
   </si>
   <si>
     <t>Posting the status</t>
+  </si>
+  <si>
+    <t>Add the news article page into Dwhomepage</t>
+  </si>
+  <si>
+    <t>NewsTitle</t>
+  </si>
+  <si>
+    <t>ShortDescription</t>
+  </si>
+  <si>
+    <t>Adding news article</t>
+  </si>
+  <si>
+    <t>News</t>
+  </si>
+  <si>
+    <t>News_Page</t>
+  </si>
+  <si>
+    <t>NewsContent</t>
+  </si>
+  <si>
+    <t>IsFeatured</t>
+  </si>
+  <si>
+    <t>PublishDate</t>
+  </si>
+  <si>
+    <t>ExpiryDate</t>
+  </si>
+  <si>
+    <t>Owner</t>
+  </si>
+  <si>
+    <t>ThumbnailImage</t>
+  </si>
+  <si>
+    <t>/PublishingImages/camper.jpg</t>
+  </si>
+  <si>
+    <t>Tags</t>
+  </si>
+  <si>
+    <t>Mentions</t>
+  </si>
+  <si>
+    <t>OrganizationalUnits</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>NewsTopic</t>
+  </si>
+  <si>
+    <t>NewsType</t>
+  </si>
+  <si>
+    <t>#newsnew</t>
+  </si>
+  <si>
+    <t>Cape Class Control Boats</t>
+  </si>
+  <si>
+    <t>Australia​</t>
+  </si>
+  <si>
+    <t>CIO​</t>
+  </si>
+  <si>
+    <t>External</t>
+  </si>
+  <si>
+    <t>30/04/2017</t>
+  </si>
+  <si>
+    <t>PublishTime</t>
+  </si>
+  <si>
+    <t>Test 05;Test 07;</t>
+  </si>
+  <si>
+    <t>News creation is completed</t>
+  </si>
+  <si>
+    <t>CheckInComments</t>
+  </si>
+  <si>
+    <t>27/03/2017</t>
+  </si>
+  <si>
+    <t>12 PM</t>
   </si>
 </sst>
 </file>
@@ -116,7 +206,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -126,6 +216,8 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -187,7 +279,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -222,7 +314,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -433,8 +525,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C1" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -473,10 +565,10 @@
         <v>8</v>
       </c>
       <c r="H1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>10</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.25">
@@ -487,22 +579,22 @@
         <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
         <v>12</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="H2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="I2" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -522,13 +614,187 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:W2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="13.5703125" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" customWidth="1"/>
+    <col min="3" max="3" width="36.7109375" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="56.7109375" customWidth="1"/>
+    <col min="6" max="6" width="27.85546875" customWidth="1"/>
+    <col min="7" max="9" width="25.42578125" customWidth="1"/>
+    <col min="10" max="10" width="20.28515625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="15.28515625" customWidth="1"/>
+    <col min="14" max="14" width="14.28515625" customWidth="1"/>
+    <col min="15" max="15" width="14.5703125" customWidth="1"/>
+    <col min="16" max="16" width="29.42578125" style="1" customWidth="1"/>
+    <col min="17" max="17" width="14.28515625" customWidth="1"/>
+    <col min="18" max="18" width="16.140625" customWidth="1"/>
+    <col min="19" max="19" width="22.85546875" customWidth="1"/>
+    <col min="20" max="20" width="12.85546875" customWidth="1"/>
+    <col min="21" max="21" width="22" customWidth="1"/>
+    <col min="22" max="22" width="16.28515625" customWidth="1"/>
+    <col min="23" max="23" width="26.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>34</v>
+      </c>
+      <c r="S2" t="s">
+        <v>35</v>
+      </c>
+      <c r="T2" t="s">
+        <v>36</v>
+      </c>
+      <c r="U2" t="s">
+        <v>37</v>
+      </c>
+      <c r="V2" t="s">
+        <v>38</v>
+      </c>
+      <c r="W2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2 K2:K1048576">
+      <formula1>"Yes,No"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2:M1048576">
+      <formula1>"12 AM,1 AM,2 AM,3 AM,4 AM,5 AM,6 AM,7 AM,8 AM,9 AM,10 AM,11 AM,12 PM,1 PM,2 PM,3 PM,4 PM,5 PM,6 PM,7 PM,8 PM,9 PM,10 PM,11 PM"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1"/>
+    <hyperlink ref="G2" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>